<commit_message>
Initial commit with correct backend/frontend structure
</commit_message>
<xml_diff>
--- a/backend/merged_property_data_cleaned.xlsx
+++ b/backend/merged_property_data_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ABDUL RAFAY\Documents\Rafay (DataBase - 2)\Job\Hema\dallas-project\dallas-commercial-map\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF6E25B-BF2C-4C5E-9D7B-B43571209763}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE6B190-06C2-41AF-93EE-1815519EBE48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22395" windowHeight="13590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5365,8 +5365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FD79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FC40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="FE54" sqref="FE54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6676,29 +6676,29 @@
       </c>
       <c r="DD3">
         <f ca="1">ROUND(228340 * (1 + (RAND() - 0.5)/10), -2)</f>
-        <v>224700</v>
+        <v>234900</v>
       </c>
       <c r="DE3" t="s">
         <v>212</v>
       </c>
       <c r="DG3">
         <f ca="1">ROUND(178340 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>190000</v>
+        <v>170000</v>
       </c>
       <c r="DL3">
         <f ca="1">ROUND(228340 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>208000</v>
+        <v>231000</v>
       </c>
       <c r="DO3">
         <f ca="1">ROUND(50000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>54000</v>
+        <v>50000</v>
       </c>
       <c r="DP3" s="5">
         <v>231850</v>
       </c>
       <c r="DQ3">
         <f ca="1">ROUND(5239.9 * (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>4991.2</v>
+        <v>4912.3</v>
       </c>
       <c r="DT3" t="s">
         <v>194</v>
@@ -7021,29 +7021,29 @@
       </c>
       <c r="DD4">
         <f t="shared" ref="DD4:DD12" ca="1" si="0">ROUND(228340 * (1 + (RAND() - 0.5)/10), -2)</f>
-        <v>235100</v>
+        <v>238200</v>
       </c>
       <c r="DE4" t="s">
         <v>212</v>
       </c>
       <c r="DG4">
         <f t="shared" ref="DG4:DG12" ca="1" si="1">ROUND(178340 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>177000</v>
+        <v>163000</v>
       </c>
       <c r="DL4">
         <f ca="1">ROUND(228340 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>221000</v>
+        <v>218000</v>
       </c>
       <c r="DO4">
         <f t="shared" ref="DO4:DO12" ca="1" si="2">ROUND(50000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>47000</v>
+        <v>51000</v>
       </c>
       <c r="DP4" s="5">
         <v>230950</v>
       </c>
       <c r="DQ4">
         <f t="shared" ref="DQ4:DQ12" ca="1" si="3">ROUND(5239.9 * (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>5662.6</v>
+        <v>5466.7</v>
       </c>
       <c r="DT4" t="s">
         <v>194</v>
@@ -7384,29 +7384,29 @@
       </c>
       <c r="DD5">
         <f t="shared" ca="1" si="0"/>
-        <v>218900</v>
+        <v>234600</v>
       </c>
       <c r="DE5" t="s">
         <v>212</v>
       </c>
       <c r="DG5">
         <f t="shared" ca="1" si="1"/>
-        <v>193000</v>
+        <v>184000</v>
       </c>
       <c r="DL5">
         <f t="shared" ref="DL5:DL12" ca="1" si="5">ROUND(228340 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>222000</v>
+        <v>240000</v>
       </c>
       <c r="DO5">
         <f t="shared" ca="1" si="2"/>
-        <v>53000</v>
+        <v>54000</v>
       </c>
       <c r="DP5" s="5">
         <v>237900</v>
       </c>
       <c r="DQ5">
         <f t="shared" ca="1" si="3"/>
-        <v>4961.8</v>
+        <v>4963.8</v>
       </c>
       <c r="DT5" t="s">
         <v>194</v>
@@ -7737,29 +7737,29 @@
       </c>
       <c r="DD6">
         <f t="shared" ca="1" si="0"/>
-        <v>232900</v>
+        <v>235100</v>
       </c>
       <c r="DE6" t="s">
         <v>212</v>
       </c>
       <c r="DG6">
         <f t="shared" ca="1" si="1"/>
-        <v>182000</v>
+        <v>190000</v>
       </c>
       <c r="DL6">
         <f t="shared" ca="1" si="5"/>
-        <v>249000</v>
+        <v>206000</v>
       </c>
       <c r="DO6">
         <f t="shared" ca="1" si="2"/>
-        <v>48000</v>
+        <v>47000</v>
       </c>
       <c r="DP6" s="6">
         <v>227300</v>
       </c>
       <c r="DQ6">
         <f t="shared" ca="1" si="3"/>
-        <v>5612.5</v>
+        <v>5599.7</v>
       </c>
       <c r="DT6" t="s">
         <v>194</v>
@@ -8097,29 +8097,29 @@
       </c>
       <c r="DD7">
         <f t="shared" ca="1" si="0"/>
-        <v>217200</v>
+        <v>230900</v>
       </c>
       <c r="DE7" t="s">
         <v>212</v>
       </c>
       <c r="DG7">
         <f t="shared" ca="1" si="1"/>
-        <v>168000</v>
+        <v>188000</v>
       </c>
       <c r="DL7">
         <f t="shared" ca="1" si="5"/>
-        <v>231000</v>
+        <v>215000</v>
       </c>
       <c r="DO7">
         <f t="shared" ca="1" si="2"/>
-        <v>47000</v>
+        <v>52000</v>
       </c>
       <c r="DP7" s="6">
         <v>231350</v>
       </c>
       <c r="DQ7">
         <f t="shared" ca="1" si="3"/>
-        <v>5150.3</v>
+        <v>4939.3999999999996</v>
       </c>
       <c r="DT7" t="s">
         <v>194</v>
@@ -8443,29 +8443,29 @@
       </c>
       <c r="DD8">
         <f t="shared" ca="1" si="0"/>
-        <v>218200</v>
+        <v>234500</v>
       </c>
       <c r="DE8" t="s">
         <v>212</v>
       </c>
       <c r="DG8">
         <f t="shared" ca="1" si="1"/>
-        <v>182000</v>
+        <v>162000</v>
       </c>
       <c r="DL8">
         <f t="shared" ca="1" si="5"/>
-        <v>250000</v>
+        <v>221000</v>
       </c>
       <c r="DO8">
         <f t="shared" ca="1" si="2"/>
-        <v>53000</v>
+        <v>51000</v>
       </c>
       <c r="DP8" s="6">
         <v>231300</v>
       </c>
       <c r="DQ8">
         <f t="shared" ca="1" si="3"/>
-        <v>5363.7</v>
+        <v>5586.6</v>
       </c>
       <c r="DT8" t="s">
         <v>194</v>
@@ -8807,29 +8807,29 @@
       </c>
       <c r="DD9">
         <f t="shared" ca="1" si="0"/>
-        <v>220500</v>
+        <v>236300</v>
       </c>
       <c r="DE9" t="s">
         <v>212</v>
       </c>
       <c r="DG9">
         <f t="shared" ca="1" si="1"/>
-        <v>162000</v>
+        <v>173000</v>
       </c>
       <c r="DL9">
         <f t="shared" ca="1" si="5"/>
-        <v>213000</v>
+        <v>222000</v>
       </c>
       <c r="DO9">
         <f t="shared" ca="1" si="2"/>
-        <v>46000</v>
+        <v>47000</v>
       </c>
       <c r="DP9" s="6">
         <v>228500</v>
       </c>
       <c r="DQ9">
         <f t="shared" ca="1" si="3"/>
-        <v>5148.1000000000004</v>
+        <v>5000.8999999999996</v>
       </c>
       <c r="DT9" t="s">
         <v>194</v>
@@ -9166,29 +9166,29 @@
       </c>
       <c r="DD10">
         <f t="shared" ca="1" si="0"/>
-        <v>219000</v>
+        <v>229900</v>
       </c>
       <c r="DE10" t="s">
         <v>212</v>
       </c>
       <c r="DG10">
         <f t="shared" ca="1" si="1"/>
-        <v>185000</v>
+        <v>171000</v>
       </c>
       <c r="DL10">
         <f t="shared" ca="1" si="5"/>
-        <v>211000</v>
+        <v>229000</v>
       </c>
       <c r="DO10">
         <f t="shared" ca="1" si="2"/>
-        <v>47000</v>
+        <v>49000</v>
       </c>
       <c r="DP10" s="6">
         <v>225700</v>
       </c>
       <c r="DQ10">
         <f t="shared" ca="1" si="3"/>
-        <v>5093</v>
+        <v>5305.4</v>
       </c>
       <c r="DT10" t="s">
         <v>194</v>
@@ -9534,29 +9534,29 @@
       </c>
       <c r="DD11">
         <f t="shared" ca="1" si="0"/>
-        <v>223000</v>
+        <v>235600</v>
       </c>
       <c r="DE11" t="s">
         <v>212</v>
       </c>
       <c r="DG11">
         <f t="shared" ca="1" si="1"/>
-        <v>179000</v>
+        <v>176000</v>
       </c>
       <c r="DL11">
         <f t="shared" ca="1" si="5"/>
-        <v>231000</v>
+        <v>219000</v>
       </c>
       <c r="DO11">
         <f t="shared" ca="1" si="2"/>
-        <v>46000</v>
+        <v>51000</v>
       </c>
       <c r="DP11" s="5">
         <v>225950</v>
       </c>
       <c r="DQ11">
         <f t="shared" ca="1" si="3"/>
-        <v>5263.6</v>
+        <v>4869.1000000000004</v>
       </c>
       <c r="DT11" t="s">
         <v>194</v>
@@ -9907,29 +9907,29 @@
       </c>
       <c r="DD12">
         <f t="shared" ca="1" si="0"/>
-        <v>224400</v>
+        <v>231900</v>
       </c>
       <c r="DE12" t="s">
         <v>212</v>
       </c>
       <c r="DG12">
         <f t="shared" ca="1" si="1"/>
-        <v>162000</v>
+        <v>165000</v>
       </c>
       <c r="DL12">
         <f t="shared" ca="1" si="5"/>
-        <v>246000</v>
+        <v>229000</v>
       </c>
       <c r="DO12">
         <f t="shared" ca="1" si="2"/>
-        <v>48000</v>
+        <v>52000</v>
       </c>
       <c r="DP12" s="5">
         <v>230750</v>
       </c>
       <c r="DQ12">
         <f t="shared" ca="1" si="3"/>
-        <v>5284.2</v>
+        <v>5248.6</v>
       </c>
       <c r="DT12" t="s">
         <v>194</v>
@@ -10726,29 +10726,29 @@
       </c>
       <c r="DD14">
         <f ca="1">ROUND(396790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>410000</v>
+        <v>390000</v>
       </c>
       <c r="DE14" t="s">
         <v>212</v>
       </c>
       <c r="DG14">
         <f ca="1">ROUND(156790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>152000</v>
+        <v>144000</v>
       </c>
       <c r="DL14">
         <f ca="1">ROUND(396790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>365000</v>
+        <v>383000</v>
       </c>
       <c r="DO14">
         <f ca="1">ROUND(240000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>251000</v>
+        <v>264000</v>
       </c>
       <c r="DP14" s="5">
         <v>216600</v>
       </c>
       <c r="DQ14">
         <f ca="1">ROUND(3959.75 * (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>3877</v>
+        <v>3985.4</v>
       </c>
     </row>
     <row r="15" spans="1:160" x14ac:dyDescent="0.25">
@@ -11012,29 +11012,29 @@
       </c>
       <c r="DD15">
         <f t="shared" ref="DD15:DD20" ca="1" si="7">ROUND(396790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>365000</v>
+        <v>410000</v>
       </c>
       <c r="DE15" t="s">
         <v>212</v>
       </c>
       <c r="DG15">
         <f t="shared" ref="DG15:DG20" ca="1" si="8">ROUND(156790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>147000</v>
+        <v>151000</v>
       </c>
       <c r="DL15">
         <f t="shared" ref="DL15:DL20" ca="1" si="9">ROUND(396790 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>433000</v>
+        <v>413000</v>
       </c>
       <c r="DO15">
         <f t="shared" ref="DO15:DO20" ca="1" si="10">ROUND(240000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>262000</v>
+        <v>234000</v>
       </c>
       <c r="DP15" s="5">
         <v>396790</v>
       </c>
       <c r="DQ15">
         <f t="shared" ref="DQ15:DQ20" ca="1" si="11">ROUND(3959.75 * (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>3611.2</v>
+        <v>4043.8</v>
       </c>
     </row>
     <row r="16" spans="1:160" x14ac:dyDescent="0.25">
@@ -11298,29 +11298,29 @@
       </c>
       <c r="DD16">
         <f t="shared" ca="1" si="7"/>
-        <v>395000</v>
+        <v>380000</v>
       </c>
       <c r="DE16" t="s">
         <v>212</v>
       </c>
       <c r="DG16">
         <f t="shared" ca="1" si="8"/>
-        <v>159000</v>
+        <v>170000</v>
       </c>
       <c r="DL16">
         <f t="shared" ca="1" si="9"/>
-        <v>382000</v>
+        <v>378000</v>
       </c>
       <c r="DO16">
         <f t="shared" ca="1" si="10"/>
-        <v>232000</v>
+        <v>259000</v>
       </c>
       <c r="DP16" s="5">
         <v>399500</v>
       </c>
       <c r="DQ16">
         <f t="shared" ca="1" si="11"/>
-        <v>3823.3</v>
+        <v>4128.8</v>
       </c>
     </row>
     <row r="17" spans="1:160" x14ac:dyDescent="0.25">
@@ -11581,18 +11581,18 @@
       </c>
       <c r="DD17">
         <f t="shared" ca="1" si="7"/>
-        <v>426000</v>
+        <v>406000</v>
       </c>
       <c r="DE17" t="s">
         <v>212</v>
       </c>
       <c r="DG17">
         <f t="shared" ca="1" si="8"/>
-        <v>144000</v>
+        <v>153000</v>
       </c>
       <c r="DL17">
         <f t="shared" ca="1" si="9"/>
-        <v>365000</v>
+        <v>421000</v>
       </c>
       <c r="DO17">
         <f t="shared" ca="1" si="10"/>
@@ -11603,7 +11603,7 @@
       </c>
       <c r="DQ17">
         <f t="shared" ca="1" si="11"/>
-        <v>3846</v>
+        <v>4332.2</v>
       </c>
     </row>
     <row r="18" spans="1:160" x14ac:dyDescent="0.25">
@@ -11861,29 +11861,29 @@
       </c>
       <c r="DD18">
         <f t="shared" ca="1" si="7"/>
-        <v>358000</v>
+        <v>394000</v>
       </c>
       <c r="DE18" t="s">
         <v>212</v>
       </c>
       <c r="DG18">
         <f t="shared" ca="1" si="8"/>
-        <v>160000</v>
+        <v>165000</v>
       </c>
       <c r="DL18">
         <f t="shared" ca="1" si="9"/>
-        <v>382000</v>
+        <v>401000</v>
       </c>
       <c r="DO18">
         <f t="shared" ca="1" si="10"/>
-        <v>231000</v>
+        <v>234000</v>
       </c>
       <c r="DP18" s="5">
         <v>409500</v>
       </c>
       <c r="DQ18">
         <f t="shared" ca="1" si="11"/>
-        <v>3647.4</v>
+        <v>4317.8</v>
       </c>
     </row>
     <row r="19" spans="1:160" x14ac:dyDescent="0.25">
@@ -12147,29 +12147,29 @@
       </c>
       <c r="DD19">
         <f t="shared" ca="1" si="7"/>
-        <v>372000</v>
+        <v>369000</v>
       </c>
       <c r="DE19" t="s">
         <v>212</v>
       </c>
       <c r="DG19">
         <f t="shared" ca="1" si="8"/>
-        <v>164000</v>
+        <v>169000</v>
       </c>
       <c r="DL19">
         <f t="shared" ca="1" si="9"/>
-        <v>404000</v>
+        <v>424000</v>
       </c>
       <c r="DO19">
         <f t="shared" ca="1" si="10"/>
-        <v>254000</v>
+        <v>233000</v>
       </c>
       <c r="DP19" s="5">
         <v>399500</v>
       </c>
       <c r="DQ19">
         <f t="shared" ca="1" si="11"/>
-        <v>4192.1000000000004</v>
+        <v>3938.4</v>
       </c>
     </row>
     <row r="20" spans="1:160" x14ac:dyDescent="0.25">
@@ -12436,29 +12436,29 @@
       </c>
       <c r="DD20">
         <f t="shared" ca="1" si="7"/>
-        <v>370000</v>
+        <v>394000</v>
       </c>
       <c r="DE20" t="s">
         <v>212</v>
       </c>
       <c r="DG20">
         <f t="shared" ca="1" si="8"/>
-        <v>143000</v>
+        <v>157000</v>
       </c>
       <c r="DL20">
         <f t="shared" ca="1" si="9"/>
-        <v>404000</v>
+        <v>420000</v>
       </c>
       <c r="DO20">
         <f t="shared" ca="1" si="10"/>
-        <v>232000</v>
+        <v>256000</v>
       </c>
       <c r="DP20" s="5">
         <v>412000</v>
       </c>
       <c r="DQ20">
         <f t="shared" ca="1" si="11"/>
-        <v>4118.6000000000004</v>
+        <v>4199.7</v>
       </c>
     </row>
     <row r="21" spans="1:160" x14ac:dyDescent="0.25">
@@ -13151,29 +13151,29 @@
       </c>
       <c r="DD22">
         <f ca="1">ROUND(225890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>214000</v>
+        <v>207000</v>
       </c>
       <c r="DE22" t="s">
         <v>212</v>
       </c>
       <c r="DG22">
         <f ca="1">ROUND(125890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>122000</v>
+        <v>121000</v>
       </c>
       <c r="DL22">
         <f ca="1">ROUND(225890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>236000</v>
+        <v>229000</v>
       </c>
       <c r="DO22">
         <f ca="1">ROUND(100000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>96000</v>
+        <v>100000</v>
       </c>
       <c r="DP22" s="5">
         <v>423500</v>
       </c>
       <c r="DQ22">
         <f ca="1">ROUND(1923.87* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>2091.6</v>
+        <v>1851.3</v>
       </c>
       <c r="DT22" t="s">
         <v>194</v>
@@ -13516,29 +13516,29 @@
       </c>
       <c r="DD23">
         <f t="shared" ref="DD23:DD35" ca="1" si="14">ROUND(225890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>207000</v>
+        <v>217000</v>
       </c>
       <c r="DE23" t="s">
         <v>212</v>
       </c>
       <c r="DG23">
         <f t="shared" ref="DG23:DG51" ca="1" si="15">ROUND(125890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>136000</v>
+        <v>115000</v>
       </c>
       <c r="DL23">
         <f t="shared" ref="DL23:DL35" ca="1" si="16">ROUND(225890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>241000</v>
+        <v>225000</v>
       </c>
       <c r="DO23">
         <f t="shared" ref="DO23:DO35" ca="1" si="17">ROUND(100000 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>92000</v>
+        <v>104000</v>
       </c>
       <c r="DP23" s="5">
         <v>225890</v>
       </c>
       <c r="DQ23">
         <f t="shared" ref="DQ23:DQ35" ca="1" si="18">ROUND(1923.87* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>1863.9</v>
+        <v>1799.8</v>
       </c>
       <c r="DT23" t="s">
         <v>194</v>
@@ -13873,29 +13873,29 @@
       </c>
       <c r="DD24">
         <f t="shared" ca="1" si="14"/>
-        <v>214000</v>
+        <v>213000</v>
       </c>
       <c r="DE24" t="s">
         <v>212</v>
       </c>
       <c r="DG24">
         <f t="shared" ca="1" si="15"/>
-        <v>115000</v>
+        <v>130000</v>
       </c>
       <c r="DL24">
         <f t="shared" ca="1" si="16"/>
-        <v>234000</v>
+        <v>211000</v>
       </c>
       <c r="DO24">
         <f t="shared" ca="1" si="17"/>
-        <v>100000</v>
+        <v>99000</v>
       </c>
       <c r="DP24" s="5">
         <v>209500</v>
       </c>
       <c r="DQ24">
         <f t="shared" ca="1" si="18"/>
-        <v>1746.6</v>
+        <v>1788.2</v>
       </c>
       <c r="DT24" t="s">
         <v>194</v>
@@ -14243,29 +14243,29 @@
       </c>
       <c r="DD25">
         <f t="shared" ca="1" si="14"/>
-        <v>207000</v>
+        <v>223000</v>
       </c>
       <c r="DE25" t="s">
         <v>212</v>
       </c>
       <c r="DG25">
         <f t="shared" ca="1" si="15"/>
-        <v>128000</v>
+        <v>129000</v>
       </c>
       <c r="DL25">
         <f t="shared" ca="1" si="16"/>
-        <v>225000</v>
+        <v>233000</v>
       </c>
       <c r="DO25">
         <f t="shared" ca="1" si="17"/>
-        <v>107000</v>
+        <v>96000</v>
       </c>
       <c r="DP25" s="5">
         <v>231500</v>
       </c>
       <c r="DQ25">
         <f t="shared" ca="1" si="18"/>
-        <v>1915.3</v>
+        <v>1775.4</v>
       </c>
       <c r="DT25" t="s">
         <v>194</v>
@@ -14619,29 +14619,29 @@
       </c>
       <c r="DD26">
         <f t="shared" ca="1" si="14"/>
-        <v>208000</v>
+        <v>214000</v>
       </c>
       <c r="DE26" t="s">
         <v>212</v>
       </c>
       <c r="DG26">
         <f t="shared" ca="1" si="15"/>
-        <v>122000</v>
+        <v>114000</v>
       </c>
       <c r="DL26">
         <f t="shared" ca="1" si="16"/>
-        <v>223000</v>
+        <v>239000</v>
       </c>
       <c r="DO26">
         <f t="shared" ca="1" si="17"/>
-        <v>103000</v>
+        <v>109000</v>
       </c>
       <c r="DP26" s="5">
         <v>223000</v>
       </c>
       <c r="DQ26">
         <f t="shared" ca="1" si="18"/>
-        <v>2073.6999999999998</v>
+        <v>2088.3000000000002</v>
       </c>
       <c r="DT26" t="s">
         <v>194</v>
@@ -14980,29 +14980,29 @@
       </c>
       <c r="DD27">
         <f t="shared" ca="1" si="14"/>
-        <v>225000</v>
+        <v>220000</v>
       </c>
       <c r="DE27" t="s">
         <v>212</v>
       </c>
       <c r="DG27">
         <f t="shared" ca="1" si="15"/>
-        <v>131000</v>
+        <v>134000</v>
       </c>
       <c r="DL27">
         <f t="shared" ca="1" si="16"/>
-        <v>215000</v>
+        <v>206000</v>
       </c>
       <c r="DO27">
         <f t="shared" ca="1" si="17"/>
-        <v>96000</v>
+        <v>95000</v>
       </c>
       <c r="DP27" s="5">
         <v>235000</v>
       </c>
       <c r="DQ27">
         <f t="shared" ca="1" si="18"/>
-        <v>1920.3</v>
+        <v>1890.3</v>
       </c>
       <c r="DT27" t="s">
         <v>194</v>
@@ -15335,29 +15335,29 @@
       </c>
       <c r="DD28">
         <f t="shared" ca="1" si="14"/>
-        <v>209000</v>
+        <v>212000</v>
       </c>
       <c r="DE28" t="s">
         <v>212</v>
       </c>
       <c r="DG28">
         <f t="shared" ca="1" si="15"/>
-        <v>120000</v>
+        <v>113000</v>
       </c>
       <c r="DL28">
         <f t="shared" ca="1" si="16"/>
-        <v>241000</v>
+        <v>209000</v>
       </c>
       <c r="DO28">
         <f t="shared" ca="1" si="17"/>
-        <v>94000</v>
+        <v>96000</v>
       </c>
       <c r="DP28" s="5">
         <v>206500</v>
       </c>
       <c r="DQ28">
         <f t="shared" ca="1" si="18"/>
-        <v>2060.4</v>
+        <v>1744</v>
       </c>
       <c r="DT28" t="s">
         <v>194</v>
@@ -15707,29 +15707,29 @@
       </c>
       <c r="DD29">
         <f t="shared" ca="1" si="14"/>
-        <v>245000</v>
+        <v>208000</v>
       </c>
       <c r="DE29" t="s">
         <v>212</v>
       </c>
       <c r="DG29">
         <f t="shared" ca="1" si="15"/>
-        <v>134000</v>
+        <v>128000</v>
       </c>
       <c r="DL29">
         <f t="shared" ca="1" si="16"/>
-        <v>211000</v>
+        <v>240000</v>
       </c>
       <c r="DO29">
         <f t="shared" ca="1" si="17"/>
-        <v>96000</v>
+        <v>104000</v>
       </c>
       <c r="DP29" s="5">
         <v>209000</v>
       </c>
       <c r="DQ29">
         <f t="shared" ca="1" si="18"/>
-        <v>1830.1</v>
+        <v>1745.5</v>
       </c>
     </row>
     <row r="30" spans="1:160" x14ac:dyDescent="0.25">
@@ -15992,29 +15992,29 @@
       </c>
       <c r="DD30">
         <f t="shared" ca="1" si="14"/>
-        <v>205000</v>
+        <v>223000</v>
       </c>
       <c r="DE30" t="s">
         <v>212</v>
       </c>
       <c r="DG30">
         <f t="shared" ca="1" si="15"/>
-        <v>121000</v>
+        <v>129000</v>
       </c>
       <c r="DL30">
         <f t="shared" ca="1" si="16"/>
-        <v>234000</v>
+        <v>239000</v>
       </c>
       <c r="DO30">
         <f t="shared" ca="1" si="17"/>
-        <v>94000</v>
+        <v>99000</v>
       </c>
       <c r="DP30" s="5">
         <v>225500</v>
       </c>
       <c r="DQ30">
         <f t="shared" ca="1" si="18"/>
-        <v>1990.1</v>
+        <v>1879.7</v>
       </c>
     </row>
     <row r="31" spans="1:160" x14ac:dyDescent="0.25">
@@ -16277,29 +16277,29 @@
       </c>
       <c r="DD31">
         <f t="shared" ca="1" si="14"/>
-        <v>209000</v>
+        <v>205000</v>
       </c>
       <c r="DE31" t="s">
         <v>212</v>
       </c>
       <c r="DG31">
         <f t="shared" ca="1" si="15"/>
-        <v>119000</v>
+        <v>135000</v>
       </c>
       <c r="DL31">
         <f t="shared" ca="1" si="16"/>
-        <v>248000</v>
+        <v>214000</v>
       </c>
       <c r="DO31">
         <f t="shared" ca="1" si="17"/>
-        <v>101000</v>
+        <v>106000</v>
       </c>
       <c r="DP31" s="5">
         <v>216000</v>
       </c>
       <c r="DQ31">
         <f t="shared" ca="1" si="18"/>
-        <v>1821.4</v>
+        <v>1794.4</v>
       </c>
     </row>
     <row r="32" spans="1:160" x14ac:dyDescent="0.25">
@@ -16545,29 +16545,29 @@
       </c>
       <c r="DD32">
         <f t="shared" ca="1" si="14"/>
-        <v>232000</v>
+        <v>223000</v>
       </c>
       <c r="DE32" t="s">
         <v>212</v>
       </c>
       <c r="DG32">
         <f t="shared" ca="1" si="15"/>
-        <v>130000</v>
+        <v>122000</v>
       </c>
       <c r="DL32">
         <f t="shared" ca="1" si="16"/>
-        <v>207000</v>
+        <v>226000</v>
       </c>
       <c r="DO32">
         <f t="shared" ca="1" si="17"/>
-        <v>105000</v>
+        <v>99000</v>
       </c>
       <c r="DP32" s="5">
         <v>219500</v>
       </c>
       <c r="DQ32">
         <f t="shared" ca="1" si="18"/>
-        <v>1971.4</v>
+        <v>1856.3</v>
       </c>
       <c r="DT32" t="s">
         <v>194</v>
@@ -16912,29 +16912,29 @@
       </c>
       <c r="DD33">
         <f t="shared" ca="1" si="14"/>
-        <v>222000</v>
+        <v>221000</v>
       </c>
       <c r="DE33" t="s">
         <v>212</v>
       </c>
       <c r="DG33">
         <f t="shared" ca="1" si="15"/>
-        <v>116000</v>
+        <v>123000</v>
       </c>
       <c r="DL33">
         <f t="shared" ca="1" si="16"/>
-        <v>211000</v>
+        <v>229000</v>
       </c>
       <c r="DO33">
         <f t="shared" ca="1" si="17"/>
-        <v>103000</v>
+        <v>104000</v>
       </c>
       <c r="DP33" s="5">
         <v>231000</v>
       </c>
       <c r="DQ33">
         <f t="shared" ca="1" si="18"/>
-        <v>1993.3</v>
+        <v>1804.7</v>
       </c>
       <c r="DT33" t="s">
         <v>194</v>
@@ -17273,29 +17273,29 @@
       </c>
       <c r="DD34">
         <f t="shared" ca="1" si="14"/>
-        <v>229000</v>
+        <v>208000</v>
       </c>
       <c r="DE34" t="s">
         <v>212</v>
       </c>
       <c r="DG34">
         <f t="shared" ca="1" si="15"/>
-        <v>126000</v>
+        <v>138000</v>
       </c>
       <c r="DL34">
         <f t="shared" ca="1" si="16"/>
-        <v>248000</v>
+        <v>204000</v>
       </c>
       <c r="DO34">
         <f t="shared" ca="1" si="17"/>
-        <v>100000</v>
+        <v>107000</v>
       </c>
       <c r="DP34" s="5">
         <v>226000</v>
       </c>
       <c r="DQ34">
         <f t="shared" ca="1" si="18"/>
-        <v>1852.7</v>
+        <v>1988.1</v>
       </c>
       <c r="DT34" t="s">
         <v>194</v>
@@ -17622,29 +17622,29 @@
       </c>
       <c r="DD35">
         <f t="shared" ca="1" si="14"/>
-        <v>238000</v>
+        <v>221000</v>
       </c>
       <c r="DE35" t="s">
         <v>212</v>
       </c>
       <c r="DG35">
         <f t="shared" ca="1" si="15"/>
-        <v>133000</v>
+        <v>136000</v>
       </c>
       <c r="DL35">
         <f t="shared" ca="1" si="16"/>
-        <v>234000</v>
+        <v>235000</v>
       </c>
       <c r="DO35">
         <f t="shared" ca="1" si="17"/>
-        <v>90000</v>
+        <v>92000</v>
       </c>
       <c r="DP35" s="5">
         <v>231000</v>
       </c>
       <c r="DQ35">
         <f t="shared" ca="1" si="18"/>
-        <v>1821.9</v>
+        <v>1878.5</v>
       </c>
       <c r="DT35" t="s">
         <v>194</v>
@@ -18420,29 +18420,29 @@
       </c>
       <c r="DD37">
         <f ca="1">ROUND(335470 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>337000</v>
+        <v>303000</v>
       </c>
       <c r="DE37" t="s">
         <v>212</v>
       </c>
       <c r="DG37">
         <f t="shared" ca="1" si="15"/>
-        <v>125000</v>
+        <v>117000</v>
       </c>
       <c r="DL37">
         <f ca="1">ROUND(335470 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>310000</v>
+        <v>309000</v>
       </c>
       <c r="DO37">
         <f ca="1">ROUND(40000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>41000</v>
+        <v>40000</v>
       </c>
       <c r="DP37" s="5">
         <v>220500</v>
       </c>
       <c r="DQ37">
         <f ca="1">ROUND(6413.45* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>6776.9</v>
+        <v>7040.4</v>
       </c>
       <c r="DT37" t="s">
         <v>194</v>
@@ -18809,29 +18809,29 @@
       </c>
       <c r="DD38">
         <f ca="1">ROUND(335470 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>313000</v>
+        <v>339000</v>
       </c>
       <c r="DE38" t="s">
         <v>212</v>
       </c>
       <c r="DG38">
         <f t="shared" ca="1" si="15"/>
-        <v>114000</v>
+        <v>138000</v>
       </c>
       <c r="DL38">
         <f ca="1">ROUND(335470 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>328000</v>
+        <v>364000</v>
       </c>
       <c r="DO38">
         <f ca="1">ROUND(40000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>37000</v>
+        <v>39000</v>
       </c>
       <c r="DP38" s="5">
         <v>335470</v>
       </c>
       <c r="DQ38">
         <f ca="1">ROUND(6413.45* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>6240.1</v>
+        <v>6625.7</v>
       </c>
       <c r="DT38" t="s">
         <v>194</v>
@@ -19586,29 +19586,29 @@
       </c>
       <c r="DD40">
         <f ca="1">ROUND(753950 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>812000</v>
+        <v>759000</v>
       </c>
       <c r="DE40" t="s">
         <v>212</v>
       </c>
       <c r="DG40">
         <f t="shared" ca="1" si="15"/>
-        <v>117000</v>
+        <v>114000</v>
       </c>
       <c r="DL40">
         <f ca="1">ROUND(753950 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>723000</v>
+        <v>742000</v>
       </c>
       <c r="DO40">
         <f ca="1">ROUND(375000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>342000</v>
+        <v>399000</v>
       </c>
       <c r="DP40" s="5">
         <v>340500</v>
       </c>
       <c r="DQ40">
         <f ca="1">ROUND(14068.14* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>14030.2</v>
+        <v>14511.4</v>
       </c>
     </row>
     <row r="41" spans="1:160" x14ac:dyDescent="0.25">
@@ -19868,29 +19868,29 @@
       </c>
       <c r="DD41">
         <f t="shared" ref="DD41:DD51" ca="1" si="21">ROUND(753950 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>722000</v>
+        <v>753000</v>
       </c>
       <c r="DE41" t="s">
         <v>212</v>
       </c>
       <c r="DG41">
         <f t="shared" ca="1" si="15"/>
-        <v>136000</v>
+        <v>130000</v>
       </c>
       <c r="DL41">
         <f t="shared" ref="DL41:DL51" ca="1" si="22">ROUND(753950 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>726000</v>
+        <v>780000</v>
       </c>
       <c r="DO41">
         <f t="shared" ref="DO41:DO51" ca="1" si="23">ROUND(375000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>362000</v>
+        <v>365000</v>
       </c>
       <c r="DP41" s="5">
         <v>753950</v>
       </c>
       <c r="DQ41">
         <f t="shared" ref="DQ41:DQ51" ca="1" si="24">ROUND(14068.14* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>14597.5</v>
+        <v>14597.3</v>
       </c>
     </row>
     <row r="42" spans="1:160" x14ac:dyDescent="0.25">
@@ -20160,29 +20160,29 @@
       </c>
       <c r="DD42">
         <f t="shared" ca="1" si="21"/>
-        <v>695000</v>
+        <v>706000</v>
       </c>
       <c r="DE42" t="s">
         <v>212</v>
       </c>
       <c r="DG42">
         <f t="shared" ca="1" si="15"/>
-        <v>136000</v>
+        <v>125000</v>
       </c>
       <c r="DL42">
         <f t="shared" ca="1" si="22"/>
-        <v>804000</v>
+        <v>695000</v>
       </c>
       <c r="DO42">
         <f t="shared" ca="1" si="23"/>
-        <v>385000</v>
+        <v>353000</v>
       </c>
       <c r="DP42" s="5">
         <v>739000</v>
       </c>
       <c r="DQ42">
         <f t="shared" ca="1" si="24"/>
-        <v>15050.4</v>
+        <v>14230</v>
       </c>
       <c r="DT42" t="s">
         <v>194</v>
@@ -20533,29 +20533,29 @@
       </c>
       <c r="DD43">
         <f t="shared" ca="1" si="21"/>
-        <v>770000</v>
+        <v>727000</v>
       </c>
       <c r="DE43" t="s">
         <v>212</v>
       </c>
       <c r="DG43">
         <f t="shared" ca="1" si="15"/>
-        <v>128000</v>
+        <v>137000</v>
       </c>
       <c r="DL43">
         <f t="shared" ca="1" si="22"/>
-        <v>826000</v>
+        <v>705000</v>
       </c>
       <c r="DO43">
         <f t="shared" ca="1" si="23"/>
-        <v>377000</v>
+        <v>406000</v>
       </c>
       <c r="DP43" s="5">
         <v>777000</v>
       </c>
       <c r="DQ43">
         <f t="shared" ca="1" si="24"/>
-        <v>13879.8</v>
+        <v>14895.6</v>
       </c>
       <c r="DT43" t="s">
         <v>194</v>
@@ -20918,29 +20918,29 @@
       </c>
       <c r="DD44">
         <f t="shared" ca="1" si="21"/>
-        <v>807000</v>
+        <v>798000</v>
       </c>
       <c r="DE44" t="s">
         <v>212</v>
       </c>
       <c r="DG44">
         <f t="shared" ca="1" si="15"/>
-        <v>132000</v>
+        <v>126000</v>
       </c>
       <c r="DL44">
         <f t="shared" ca="1" si="22"/>
-        <v>761000</v>
+        <v>686000</v>
       </c>
       <c r="DO44">
         <f t="shared" ca="1" si="23"/>
-        <v>350000</v>
+        <v>385000</v>
       </c>
       <c r="DP44" s="5">
         <v>737000</v>
       </c>
       <c r="DQ44">
         <f t="shared" ca="1" si="24"/>
-        <v>15115</v>
+        <v>15315.9</v>
       </c>
       <c r="DT44" t="s">
         <v>194</v>
@@ -21293,29 +21293,29 @@
       </c>
       <c r="DD45">
         <f t="shared" ca="1" si="21"/>
-        <v>688000</v>
+        <v>697000</v>
       </c>
       <c r="DE45" t="s">
         <v>212</v>
       </c>
       <c r="DG45">
         <f t="shared" ca="1" si="15"/>
-        <v>130000</v>
+        <v>119000</v>
       </c>
       <c r="DL45">
         <f t="shared" ca="1" si="22"/>
-        <v>709000</v>
+        <v>798000</v>
       </c>
       <c r="DO45">
         <f t="shared" ca="1" si="23"/>
-        <v>373000</v>
+        <v>395000</v>
       </c>
       <c r="DP45" s="5">
         <v>785500</v>
       </c>
       <c r="DQ45">
         <f t="shared" ca="1" si="24"/>
-        <v>13275.3</v>
+        <v>14173.7</v>
       </c>
       <c r="DT45" t="s">
         <v>194</v>
@@ -21651,29 +21651,29 @@
       </c>
       <c r="DD46">
         <f t="shared" ca="1" si="21"/>
-        <v>790000</v>
+        <v>713000</v>
       </c>
       <c r="DE46" t="s">
         <v>212</v>
       </c>
       <c r="DG46">
         <f t="shared" ca="1" si="15"/>
-        <v>134000</v>
+        <v>124000</v>
       </c>
       <c r="DL46">
         <f t="shared" ca="1" si="22"/>
-        <v>681000</v>
+        <v>763000</v>
       </c>
       <c r="DO46">
         <f t="shared" ca="1" si="23"/>
-        <v>345000</v>
+        <v>402000</v>
       </c>
       <c r="DP46" s="5">
         <v>720500</v>
       </c>
       <c r="DQ46">
         <f t="shared" ca="1" si="24"/>
-        <v>13518.9</v>
+        <v>13063.5</v>
       </c>
       <c r="DT46" t="s">
         <v>194</v>
@@ -21996,29 +21996,29 @@
       </c>
       <c r="DD47">
         <f t="shared" ca="1" si="21"/>
-        <v>773000</v>
+        <v>701000</v>
       </c>
       <c r="DE47" t="s">
         <v>212</v>
       </c>
       <c r="DG47">
         <f t="shared" ca="1" si="15"/>
-        <v>125000</v>
+        <v>137000</v>
       </c>
       <c r="DL47">
         <f t="shared" ca="1" si="22"/>
-        <v>794000</v>
+        <v>682000</v>
       </c>
       <c r="DO47">
         <f t="shared" ca="1" si="23"/>
-        <v>395000</v>
+        <v>348000</v>
       </c>
       <c r="DP47" s="5">
         <v>764000</v>
       </c>
       <c r="DQ47">
         <f t="shared" ca="1" si="24"/>
-        <v>14574.1</v>
+        <v>13835.7</v>
       </c>
     </row>
     <row r="48" spans="1:160" x14ac:dyDescent="0.25">
@@ -22285,29 +22285,29 @@
       </c>
       <c r="DD48">
         <f t="shared" ca="1" si="21"/>
-        <v>711000</v>
+        <v>680000</v>
       </c>
       <c r="DE48" t="s">
         <v>212</v>
       </c>
       <c r="DG48">
         <f t="shared" ca="1" si="15"/>
-        <v>126000</v>
+        <v>135000</v>
       </c>
       <c r="DL48">
         <f t="shared" ca="1" si="22"/>
-        <v>784000</v>
+        <v>756000</v>
       </c>
       <c r="DO48">
         <f t="shared" ca="1" si="23"/>
-        <v>349000</v>
+        <v>406000</v>
       </c>
       <c r="DP48" s="5">
         <v>787000</v>
       </c>
       <c r="DQ48">
         <f t="shared" ca="1" si="24"/>
-        <v>13118.6</v>
+        <v>13797.2</v>
       </c>
       <c r="DT48" t="s">
         <v>194</v>
@@ -22670,29 +22670,29 @@
       </c>
       <c r="DD49">
         <f t="shared" ca="1" si="21"/>
-        <v>815000</v>
+        <v>776000</v>
       </c>
       <c r="DE49" t="s">
         <v>212</v>
       </c>
       <c r="DG49">
         <f t="shared" ca="1" si="15"/>
-        <v>115000</v>
+        <v>122000</v>
       </c>
       <c r="DL49">
         <f t="shared" ca="1" si="22"/>
-        <v>711000</v>
+        <v>778000</v>
       </c>
       <c r="DO49">
         <f t="shared" ca="1" si="23"/>
-        <v>395000</v>
+        <v>376000</v>
       </c>
       <c r="DP49" s="5">
         <v>772000</v>
       </c>
       <c r="DQ49">
         <f t="shared" ca="1" si="24"/>
-        <v>12828.2</v>
+        <v>12977.5</v>
       </c>
       <c r="DT49" t="s">
         <v>194</v>
@@ -23034,29 +23034,29 @@
       </c>
       <c r="DD50">
         <f t="shared" ca="1" si="21"/>
-        <v>714000</v>
+        <v>751000</v>
       </c>
       <c r="DE50" t="s">
         <v>212</v>
       </c>
       <c r="DG50">
         <f t="shared" ca="1" si="15"/>
-        <v>138000</v>
+        <v>128000</v>
       </c>
       <c r="DL50">
         <f t="shared" ca="1" si="22"/>
-        <v>804000</v>
+        <v>691000</v>
       </c>
       <c r="DO50">
         <f t="shared" ca="1" si="23"/>
-        <v>394000</v>
+        <v>360000</v>
       </c>
       <c r="DP50" s="5">
         <v>700500</v>
       </c>
       <c r="DQ50">
         <f t="shared" ca="1" si="24"/>
-        <v>15166.7</v>
+        <v>14200.6</v>
       </c>
       <c r="DT50" t="s">
         <v>194</v>
@@ -23407,29 +23407,29 @@
       </c>
       <c r="DD51">
         <f t="shared" ca="1" si="21"/>
-        <v>704000</v>
+        <v>773000</v>
       </c>
       <c r="DE51" t="s">
         <v>212</v>
       </c>
       <c r="DG51">
         <f t="shared" ca="1" si="15"/>
-        <v>117000</v>
+        <v>120000</v>
       </c>
       <c r="DL51">
         <f t="shared" ca="1" si="22"/>
-        <v>806000</v>
+        <v>801000</v>
       </c>
       <c r="DO51">
         <f t="shared" ca="1" si="23"/>
-        <v>383000</v>
+        <v>376000</v>
       </c>
       <c r="DP51" s="5">
         <v>697000</v>
       </c>
       <c r="DQ51">
         <f t="shared" ca="1" si="24"/>
-        <v>14737.3</v>
+        <v>14970.1</v>
       </c>
       <c r="DT51" t="s">
         <v>194</v>
@@ -24599,29 +24599,29 @@
       </c>
       <c r="DD54">
         <f ca="1">ROUND(422890 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>416000</v>
+        <v>451000</v>
       </c>
       <c r="DE54" t="s">
         <v>212</v>
       </c>
       <c r="DG54">
         <f ca="1">ROUND(347890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>377000</v>
+        <v>334000</v>
       </c>
       <c r="DL54">
         <f ca="1">ROUND(422890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>417000</v>
+        <v>403000</v>
       </c>
       <c r="DO54">
         <f ca="1">ROUND(75000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>78000</v>
+        <v>77000</v>
       </c>
       <c r="DP54" s="5">
         <v>764000</v>
       </c>
       <c r="DQ54">
         <f ca="1">ROUND(7157.26* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>6544.1</v>
+        <v>7445.8</v>
       </c>
       <c r="DT54" t="s">
         <v>194</v>
@@ -24963,29 +24963,29 @@
       </c>
       <c r="DD55">
         <f t="shared" ref="DD55:DD62" ca="1" si="25">ROUND(422890 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>434000</v>
+        <v>433000</v>
       </c>
       <c r="DE55" t="s">
         <v>212</v>
       </c>
       <c r="DG55">
         <f t="shared" ref="DG55:DG62" ca="1" si="26">ROUND(347890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>332000</v>
+        <v>349000</v>
       </c>
       <c r="DL55">
         <f t="shared" ref="DL55:DL62" ca="1" si="27">ROUND(422890 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>400000</v>
+        <v>406000</v>
       </c>
       <c r="DO55">
         <f t="shared" ref="DO55:DO62" ca="1" si="28">ROUND(75000* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>71000</v>
+        <v>78000</v>
       </c>
       <c r="DP55" s="5">
         <v>702500</v>
       </c>
       <c r="DQ55">
         <f t="shared" ref="DQ55:DQ62" ca="1" si="29">ROUND(7157.26* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>7464.2</v>
+        <v>6442.6</v>
       </c>
       <c r="DT55" t="s">
         <v>194</v>
@@ -25310,29 +25310,29 @@
       </c>
       <c r="DD56">
         <f t="shared" ca="1" si="25"/>
-        <v>460000</v>
+        <v>419000</v>
       </c>
       <c r="DE56" t="s">
         <v>212</v>
       </c>
       <c r="DG56">
         <f t="shared" ca="1" si="26"/>
-        <v>378000</v>
+        <v>353000</v>
       </c>
       <c r="DL56">
         <f t="shared" ca="1" si="27"/>
-        <v>383000</v>
+        <v>465000</v>
       </c>
       <c r="DO56">
         <f t="shared" ca="1" si="28"/>
-        <v>80000</v>
+        <v>76000</v>
       </c>
       <c r="DP56" s="5">
         <v>529800</v>
       </c>
       <c r="DQ56">
         <f t="shared" ca="1" si="29"/>
-        <v>6623.3</v>
+        <v>6809.5</v>
       </c>
       <c r="DT56" t="s">
         <v>194</v>
@@ -25680,29 +25680,29 @@
       </c>
       <c r="DD57">
         <f t="shared" ca="1" si="25"/>
-        <v>465000</v>
+        <v>444000</v>
       </c>
       <c r="DE57" t="s">
         <v>212</v>
       </c>
       <c r="DG57">
         <f t="shared" ca="1" si="26"/>
-        <v>381000</v>
+        <v>368000</v>
       </c>
       <c r="DL57">
         <f t="shared" ca="1" si="27"/>
-        <v>440000</v>
+        <v>437000</v>
       </c>
       <c r="DO57">
         <f t="shared" ca="1" si="28"/>
-        <v>78000</v>
+        <v>68000</v>
       </c>
       <c r="DP57" s="5">
         <v>422890</v>
       </c>
       <c r="DQ57">
         <f t="shared" ca="1" si="29"/>
-        <v>7694.8</v>
+        <v>7834.9</v>
       </c>
       <c r="DT57" t="s">
         <v>194</v>
@@ -26053,18 +26053,18 @@
       </c>
       <c r="DD58">
         <f t="shared" ca="1" si="25"/>
-        <v>421000</v>
+        <v>384000</v>
       </c>
       <c r="DE58" t="s">
         <v>212</v>
       </c>
       <c r="DG58">
         <f t="shared" ca="1" si="26"/>
-        <v>350000</v>
+        <v>362000</v>
       </c>
       <c r="DL58">
         <f t="shared" ca="1" si="27"/>
-        <v>431000</v>
+        <v>416000</v>
       </c>
       <c r="DO58">
         <f t="shared" ca="1" si="28"/>
@@ -26075,7 +26075,7 @@
       </c>
       <c r="DQ58">
         <f t="shared" ca="1" si="29"/>
-        <v>7567.5</v>
+        <v>6891.9</v>
       </c>
       <c r="DT58" t="s">
         <v>194</v>
@@ -26417,14 +26417,14 @@
       </c>
       <c r="DD59">
         <f t="shared" ca="1" si="25"/>
-        <v>459000</v>
+        <v>446000</v>
       </c>
       <c r="DE59" t="s">
         <v>212</v>
       </c>
       <c r="DG59">
         <f t="shared" ca="1" si="26"/>
-        <v>332000</v>
+        <v>347000</v>
       </c>
       <c r="DL59">
         <f t="shared" ca="1" si="27"/>
@@ -26432,14 +26432,14 @@
       </c>
       <c r="DO59">
         <f t="shared" ca="1" si="28"/>
-        <v>78000</v>
+        <v>81000</v>
       </c>
       <c r="DP59" s="5">
         <v>424500</v>
       </c>
       <c r="DQ59">
         <f t="shared" ca="1" si="29"/>
-        <v>6970.4</v>
+        <v>7214.2</v>
       </c>
       <c r="DT59" t="s">
         <v>194</v>
@@ -26778,29 +26778,29 @@
       </c>
       <c r="DD60">
         <f t="shared" ca="1" si="25"/>
-        <v>414000</v>
+        <v>422000</v>
       </c>
       <c r="DE60" t="s">
         <v>212</v>
       </c>
       <c r="DG60">
         <f t="shared" ca="1" si="26"/>
-        <v>370000</v>
+        <v>352000</v>
       </c>
       <c r="DL60">
         <f t="shared" ca="1" si="27"/>
-        <v>383000</v>
+        <v>447000</v>
       </c>
       <c r="DO60">
         <f t="shared" ca="1" si="28"/>
-        <v>70000</v>
+        <v>79000</v>
       </c>
       <c r="DP60" s="5">
         <v>446000</v>
       </c>
       <c r="DQ60">
         <f t="shared" ca="1" si="29"/>
-        <v>6477.1</v>
+        <v>7707.4</v>
       </c>
       <c r="DT60" t="s">
         <v>194</v>
@@ -27133,29 +27133,29 @@
       </c>
       <c r="DD61">
         <f t="shared" ca="1" si="25"/>
-        <v>401000</v>
+        <v>404000</v>
       </c>
       <c r="DE61" t="s">
         <v>212</v>
       </c>
       <c r="DG61">
         <f t="shared" ca="1" si="26"/>
-        <v>373000</v>
+        <v>321000</v>
       </c>
       <c r="DL61">
         <f t="shared" ca="1" si="27"/>
-        <v>463000</v>
+        <v>438000</v>
       </c>
       <c r="DO61">
         <f t="shared" ca="1" si="28"/>
-        <v>72000</v>
+        <v>71000</v>
       </c>
       <c r="DP61" s="5">
         <v>414000</v>
       </c>
       <c r="DQ61">
         <f t="shared" ca="1" si="29"/>
-        <v>6810</v>
+        <v>6928.8</v>
       </c>
     </row>
     <row r="62" spans="1:160" x14ac:dyDescent="0.25">
@@ -27419,29 +27419,29 @@
       </c>
       <c r="DD62">
         <f t="shared" ca="1" si="25"/>
-        <v>459000</v>
+        <v>423000</v>
       </c>
       <c r="DE62" t="s">
         <v>212</v>
       </c>
       <c r="DG62">
         <f t="shared" ca="1" si="26"/>
-        <v>359000</v>
+        <v>352000</v>
       </c>
       <c r="DL62">
         <f t="shared" ca="1" si="27"/>
-        <v>438000</v>
+        <v>385000</v>
       </c>
       <c r="DO62">
         <f t="shared" ca="1" si="28"/>
-        <v>68000</v>
+        <v>78000</v>
       </c>
       <c r="DP62" s="5">
         <v>438500</v>
       </c>
       <c r="DQ62">
         <f t="shared" ca="1" si="29"/>
-        <v>7489.5</v>
+        <v>7183.1</v>
       </c>
       <c r="DT62" t="s">
         <v>194</v>
@@ -28217,29 +28217,29 @@
       </c>
       <c r="DD64">
         <f ca="1">ROUND(662980 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>650000</v>
+        <v>631000</v>
       </c>
       <c r="DE64" t="s">
         <v>212</v>
       </c>
       <c r="DG64">
         <f ca="1">ROUND(194330 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>205000</v>
+        <v>186000</v>
       </c>
       <c r="DL64">
         <f ca="1">ROUND(662980 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>676000</v>
+        <v>709000</v>
       </c>
       <c r="DO64">
         <f ca="1">ROUND(468650* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>493000</v>
+        <v>430000</v>
       </c>
       <c r="DP64" s="5">
         <v>439000</v>
       </c>
       <c r="DQ64">
         <f ca="1">ROUND(10027.74* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>11018.8</v>
+        <v>10635.4</v>
       </c>
       <c r="DT64" t="s">
         <v>194</v>
@@ -28573,29 +28573,29 @@
       </c>
       <c r="DD65">
         <f t="shared" ref="DD65:DD76" ca="1" si="30">ROUND(662980 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>697000</v>
+        <v>645000</v>
       </c>
       <c r="DE65" t="s">
         <v>212</v>
       </c>
       <c r="DG65">
         <f t="shared" ref="DG65:DG79" ca="1" si="31">ROUND(194330 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>188000</v>
+        <v>181000</v>
       </c>
       <c r="DL65">
         <f t="shared" ref="DL65:DL79" ca="1" si="32">ROUND(662980 * (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>666000</v>
+        <v>650000</v>
       </c>
       <c r="DO65">
         <f t="shared" ref="DO65:DO79" ca="1" si="33">ROUND(468650* (1 + (RAND() - 0.5)/5), -3)</f>
-        <v>431000</v>
+        <v>428000</v>
       </c>
       <c r="DP65" s="5">
         <v>440500</v>
       </c>
       <c r="DQ65">
         <f t="shared" ref="DQ65:DQ79" ca="1" si="34">ROUND(10027.74* (1 + (RAND() - 0.5)/5), 1)</f>
-        <v>9051.9</v>
+        <v>9438.7999999999993</v>
       </c>
     </row>
     <row r="66" spans="1:160" x14ac:dyDescent="0.25">
@@ -28856,29 +28856,29 @@
       </c>
       <c r="DD66">
         <f t="shared" ca="1" si="30"/>
-        <v>713000</v>
+        <v>606000</v>
       </c>
       <c r="DE66" t="s">
         <v>212</v>
       </c>
       <c r="DG66">
         <f t="shared" ca="1" si="31"/>
-        <v>185000</v>
+        <v>175000</v>
       </c>
       <c r="DL66">
         <f t="shared" ca="1" si="32"/>
-        <v>680000</v>
+        <v>603000</v>
       </c>
       <c r="DO66">
         <f t="shared" ca="1" si="33"/>
-        <v>474000</v>
+        <v>496000</v>
       </c>
       <c r="DP66" s="5">
         <v>421500</v>
       </c>
       <c r="DQ66">
         <f t="shared" ca="1" si="34"/>
-        <v>9504.5</v>
+        <v>9986.6</v>
       </c>
       <c r="DT66" t="s">
         <v>194</v>
@@ -29217,29 +29217,29 @@
       </c>
       <c r="DD67">
         <f t="shared" ca="1" si="30"/>
-        <v>618000</v>
+        <v>632000</v>
       </c>
       <c r="DE67" t="s">
         <v>212</v>
       </c>
       <c r="DG67">
         <f t="shared" ca="1" si="31"/>
-        <v>189000</v>
+        <v>201000</v>
       </c>
       <c r="DL67">
         <f t="shared" ca="1" si="32"/>
-        <v>681000</v>
+        <v>652000</v>
       </c>
       <c r="DO67">
         <f t="shared" ca="1" si="33"/>
-        <v>464000</v>
+        <v>424000</v>
       </c>
       <c r="DP67" s="5">
         <v>418500</v>
       </c>
       <c r="DQ67">
         <f t="shared" ca="1" si="34"/>
-        <v>10538</v>
+        <v>10963.3</v>
       </c>
       <c r="DT67" t="s">
         <v>194</v>
@@ -29596,29 +29596,29 @@
       </c>
       <c r="DD68">
         <f t="shared" ca="1" si="30"/>
-        <v>674000</v>
+        <v>725000</v>
       </c>
       <c r="DE68" t="s">
         <v>212</v>
       </c>
       <c r="DG68">
         <f t="shared" ca="1" si="31"/>
-        <v>189000</v>
+        <v>175000</v>
       </c>
       <c r="DL68">
         <f t="shared" ca="1" si="32"/>
-        <v>676000</v>
+        <v>638000</v>
       </c>
       <c r="DO68">
         <f t="shared" ca="1" si="33"/>
-        <v>514000</v>
+        <v>457000</v>
       </c>
       <c r="DP68" s="5">
         <v>662980</v>
       </c>
       <c r="DQ68">
         <f t="shared" ca="1" si="34"/>
-        <v>9367.4</v>
+        <v>9661.7999999999993</v>
       </c>
       <c r="DT68" t="s">
         <v>194</v>
@@ -29942,29 +29942,29 @@
       </c>
       <c r="DD69">
         <f t="shared" ca="1" si="30"/>
-        <v>663000</v>
+        <v>680000</v>
       </c>
       <c r="DE69" t="s">
         <v>212</v>
       </c>
       <c r="DG69">
         <f t="shared" ca="1" si="31"/>
-        <v>208000</v>
+        <v>186000</v>
       </c>
       <c r="DL69">
         <f t="shared" ca="1" si="32"/>
-        <v>614000</v>
+        <v>634000</v>
       </c>
       <c r="DO69">
         <f t="shared" ca="1" si="33"/>
-        <v>485000</v>
+        <v>472000</v>
       </c>
       <c r="DP69" s="5">
         <v>708000</v>
       </c>
       <c r="DQ69">
         <f t="shared" ca="1" si="34"/>
-        <v>9466.2000000000007</v>
+        <v>10531.8</v>
       </c>
       <c r="DT69" t="s">
         <v>194</v>
@@ -30309,29 +30309,29 @@
       </c>
       <c r="DD70">
         <f t="shared" ca="1" si="30"/>
-        <v>620000</v>
+        <v>667000</v>
       </c>
       <c r="DE70" t="s">
         <v>212</v>
       </c>
       <c r="DG70">
         <f t="shared" ca="1" si="31"/>
-        <v>187000</v>
+        <v>214000</v>
       </c>
       <c r="DL70">
         <f t="shared" ca="1" si="32"/>
-        <v>648000</v>
+        <v>654000</v>
       </c>
       <c r="DO70">
         <f t="shared" ca="1" si="33"/>
-        <v>446000</v>
+        <v>452000</v>
       </c>
       <c r="DP70" s="5">
         <v>695000</v>
       </c>
       <c r="DQ70">
         <f t="shared" ca="1" si="34"/>
-        <v>9621.4</v>
+        <v>9724.1</v>
       </c>
       <c r="DU70" t="s">
         <v>269</v>
@@ -30670,29 +30670,29 @@
       </c>
       <c r="DD71">
         <f t="shared" ca="1" si="30"/>
-        <v>700000</v>
+        <v>667000</v>
       </c>
       <c r="DE71" t="s">
         <v>212</v>
       </c>
       <c r="DG71">
         <f t="shared" ca="1" si="31"/>
-        <v>186000</v>
+        <v>210000</v>
       </c>
       <c r="DL71">
         <f t="shared" ca="1" si="32"/>
-        <v>716000</v>
+        <v>697000</v>
       </c>
       <c r="DO71">
         <f t="shared" ca="1" si="33"/>
-        <v>448000</v>
+        <v>465000</v>
       </c>
       <c r="DP71" s="5">
         <v>672000</v>
       </c>
       <c r="DQ71">
         <f t="shared" ca="1" si="34"/>
-        <v>9226.2000000000007</v>
+        <v>9857.7999999999993</v>
       </c>
       <c r="DT71" t="s">
         <v>194</v>
@@ -31043,29 +31043,29 @@
       </c>
       <c r="DD72">
         <f t="shared" ca="1" si="30"/>
-        <v>639000</v>
+        <v>621000</v>
       </c>
       <c r="DE72" t="s">
         <v>212</v>
       </c>
       <c r="DG72">
         <f t="shared" ca="1" si="31"/>
-        <v>188000</v>
+        <v>197000</v>
       </c>
       <c r="DL72">
         <f t="shared" ca="1" si="32"/>
-        <v>723000</v>
+        <v>674000</v>
       </c>
       <c r="DO72">
         <f t="shared" ca="1" si="33"/>
-        <v>448000</v>
+        <v>472000</v>
       </c>
       <c r="DP72" s="5">
         <v>645000</v>
       </c>
       <c r="DQ72">
         <f t="shared" ca="1" si="34"/>
-        <v>10458.6</v>
+        <v>10700.8</v>
       </c>
       <c r="DT72" t="s">
         <v>194</v>
@@ -31407,29 +31407,29 @@
       </c>
       <c r="DD73">
         <f t="shared" ca="1" si="30"/>
-        <v>673000</v>
+        <v>653000</v>
       </c>
       <c r="DE73" t="s">
         <v>212</v>
       </c>
       <c r="DG73">
         <f t="shared" ca="1" si="31"/>
-        <v>180000</v>
+        <v>195000</v>
       </c>
       <c r="DL73">
         <f t="shared" ca="1" si="32"/>
-        <v>650000</v>
+        <v>620000</v>
       </c>
       <c r="DO73">
         <f t="shared" ca="1" si="33"/>
-        <v>481000</v>
+        <v>424000</v>
       </c>
       <c r="DP73" s="5">
         <v>669000</v>
       </c>
       <c r="DQ73">
         <f t="shared" ca="1" si="34"/>
-        <v>10207.4</v>
+        <v>10658.2</v>
       </c>
       <c r="DT73" t="s">
         <v>194</v>
@@ -31777,29 +31777,29 @@
       </c>
       <c r="DD74">
         <f ca="1">ROUND(662980 * (1 + (RAND() - 0.5)/5),-3)</f>
-        <v>611000</v>
+        <v>627000</v>
       </c>
       <c r="DE74" t="s">
         <v>212</v>
       </c>
       <c r="DG74">
         <f t="shared" ca="1" si="31"/>
-        <v>180000</v>
+        <v>211000</v>
       </c>
       <c r="DL74">
         <f t="shared" ca="1" si="32"/>
-        <v>695000</v>
+        <v>625000</v>
       </c>
       <c r="DO74">
         <f t="shared" ca="1" si="33"/>
-        <v>487000</v>
+        <v>485000</v>
       </c>
       <c r="DP74" s="5">
         <v>665000</v>
       </c>
       <c r="DQ74">
         <f t="shared" ca="1" si="34"/>
-        <v>10761.7</v>
+        <v>10005.5</v>
       </c>
       <c r="DT74" t="s">
         <v>194</v>
@@ -32099,29 +32099,29 @@
       </c>
       <c r="DD75">
         <f t="shared" ca="1" si="30"/>
-        <v>607000</v>
+        <v>609000</v>
       </c>
       <c r="DE75" t="s">
         <v>212</v>
       </c>
       <c r="DG75">
         <f t="shared" ca="1" si="31"/>
-        <v>207000</v>
+        <v>200000</v>
       </c>
       <c r="DL75">
         <f t="shared" ca="1" si="32"/>
-        <v>635000</v>
+        <v>721000</v>
       </c>
       <c r="DO75">
         <f t="shared" ca="1" si="33"/>
-        <v>498000</v>
+        <v>504000</v>
       </c>
       <c r="DP75" s="5">
         <v>664500</v>
       </c>
       <c r="DQ75">
         <f t="shared" ca="1" si="34"/>
-        <v>10186.299999999999</v>
+        <v>10673.8</v>
       </c>
     </row>
     <row r="76" spans="1:160" x14ac:dyDescent="0.25">
@@ -32376,29 +32376,29 @@
       </c>
       <c r="DD76">
         <f t="shared" ca="1" si="30"/>
-        <v>708000</v>
+        <v>691000</v>
       </c>
       <c r="DE76" t="s">
         <v>212</v>
       </c>
       <c r="DG76">
         <f t="shared" ca="1" si="31"/>
-        <v>183000</v>
+        <v>193000</v>
       </c>
       <c r="DL76">
         <f t="shared" ca="1" si="32"/>
-        <v>680000</v>
+        <v>728000</v>
       </c>
       <c r="DO76">
         <f t="shared" ca="1" si="33"/>
-        <v>510000</v>
+        <v>457000</v>
       </c>
       <c r="DP76" s="5">
         <v>687500</v>
       </c>
       <c r="DQ76">
         <f t="shared" ca="1" si="34"/>
-        <v>9168.9</v>
+        <v>10777</v>
       </c>
       <c r="DT76" t="s">
         <v>194</v>
@@ -32739,22 +32739,22 @@
       </c>
       <c r="DG77">
         <f t="shared" ca="1" si="31"/>
-        <v>178000</v>
+        <v>207000</v>
       </c>
       <c r="DL77">
         <f t="shared" ca="1" si="32"/>
-        <v>640000</v>
+        <v>611000</v>
       </c>
       <c r="DO77">
         <f t="shared" ca="1" si="33"/>
-        <v>502000</v>
+        <v>493000</v>
       </c>
       <c r="DP77" s="5">
         <v>687500</v>
       </c>
       <c r="DQ77">
         <f t="shared" ca="1" si="34"/>
-        <v>9503.2999999999993</v>
+        <v>10465.799999999999</v>
       </c>
     </row>
     <row r="78" spans="1:160" x14ac:dyDescent="0.25">
@@ -33018,22 +33018,22 @@
       </c>
       <c r="DG78">
         <f t="shared" ca="1" si="31"/>
-        <v>185000</v>
+        <v>191000</v>
       </c>
       <c r="DL78">
         <f t="shared" ca="1" si="32"/>
-        <v>650000</v>
+        <v>687000</v>
       </c>
       <c r="DO78">
         <f t="shared" ca="1" si="33"/>
-        <v>453000</v>
+        <v>460000</v>
       </c>
       <c r="DP78" s="5">
         <v>687500</v>
       </c>
       <c r="DQ78">
         <f t="shared" ca="1" si="34"/>
-        <v>10393.799999999999</v>
+        <v>10792.3</v>
       </c>
     </row>
     <row r="79" spans="1:160" x14ac:dyDescent="0.25">
@@ -33297,22 +33297,22 @@
       </c>
       <c r="DG79">
         <f t="shared" ca="1" si="31"/>
-        <v>176000</v>
+        <v>185000</v>
       </c>
       <c r="DL79">
         <f t="shared" ca="1" si="32"/>
-        <v>702000</v>
+        <v>601000</v>
       </c>
       <c r="DO79">
         <f t="shared" ca="1" si="33"/>
-        <v>511000</v>
+        <v>495000</v>
       </c>
       <c r="DP79" s="5">
         <v>687500</v>
       </c>
       <c r="DQ79">
         <f t="shared" ca="1" si="34"/>
-        <v>10966.1</v>
+        <v>9297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>